<commit_message>
update ratings employee ratings table
</commit_message>
<xml_diff>
--- a/Examples/AHP_Ratings_Employee_Evaluation/Ratings_Employee_Eval_ratingstable.xlsx
+++ b/Examples/AHP_Ratings_Employee_Evaluation/Ratings_Employee_Eval_ratingstable.xlsx
@@ -2698,7 +2698,217 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="35">
+  <dataValidations count="105">
+    <dataValidation sqref="B2" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A3:A7</formula1>
+    </dataValidation>
+    <dataValidation sqref="B3" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A3:A7</formula1>
+    </dataValidation>
+    <dataValidation sqref="B4" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A3:A7</formula1>
+    </dataValidation>
+    <dataValidation sqref="B5" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A3:A7</formula1>
+    </dataValidation>
+    <dataValidation sqref="B6" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A3:A7</formula1>
+    </dataValidation>
+    <dataValidation sqref="C2" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A13:A16</formula1>
+    </dataValidation>
+    <dataValidation sqref="C3" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A13:A16</formula1>
+    </dataValidation>
+    <dataValidation sqref="C4" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A13:A16</formula1>
+    </dataValidation>
+    <dataValidation sqref="C5" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A13:A16</formula1>
+    </dataValidation>
+    <dataValidation sqref="C6" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A13:A16</formula1>
+    </dataValidation>
+    <dataValidation sqref="D2" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A22:A25</formula1>
+    </dataValidation>
+    <dataValidation sqref="D3" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A22:A25</formula1>
+    </dataValidation>
+    <dataValidation sqref="D4" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A22:A25</formula1>
+    </dataValidation>
+    <dataValidation sqref="D5" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A22:A25</formula1>
+    </dataValidation>
+    <dataValidation sqref="D6" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A22:A25</formula1>
+    </dataValidation>
+    <dataValidation sqref="E2" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A31:A34</formula1>
+    </dataValidation>
+    <dataValidation sqref="E3" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A31:A34</formula1>
+    </dataValidation>
+    <dataValidation sqref="E4" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A31:A34</formula1>
+    </dataValidation>
+    <dataValidation sqref="E5" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A31:A34</formula1>
+    </dataValidation>
+    <dataValidation sqref="E6" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A31:A34</formula1>
+    </dataValidation>
+    <dataValidation sqref="F2" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A40:A44</formula1>
+    </dataValidation>
+    <dataValidation sqref="F3" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A40:A44</formula1>
+    </dataValidation>
+    <dataValidation sqref="F4" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A40:A44</formula1>
+    </dataValidation>
+    <dataValidation sqref="F5" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A40:A44</formula1>
+    </dataValidation>
+    <dataValidation sqref="F6" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A40:A44</formula1>
+    </dataValidation>
+    <dataValidation sqref="G2" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A50:A53</formula1>
+    </dataValidation>
+    <dataValidation sqref="G3" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A50:A53</formula1>
+    </dataValidation>
+    <dataValidation sqref="G4" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A50:A53</formula1>
+    </dataValidation>
+    <dataValidation sqref="G5" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A50:A53</formula1>
+    </dataValidation>
+    <dataValidation sqref="G6" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A50:A53</formula1>
+    </dataValidation>
+    <dataValidation sqref="H2" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A59:A62</formula1>
+    </dataValidation>
+    <dataValidation sqref="H3" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A59:A62</formula1>
+    </dataValidation>
+    <dataValidation sqref="H4" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A59:A62</formula1>
+    </dataValidation>
+    <dataValidation sqref="H5" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A59:A62</formula1>
+    </dataValidation>
+    <dataValidation sqref="H6" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A59:A62</formula1>
+    </dataValidation>
+    <dataValidation sqref="B2" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A3:A7</formula1>
+    </dataValidation>
+    <dataValidation sqref="B3" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A3:A7</formula1>
+    </dataValidation>
+    <dataValidation sqref="B4" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A3:A7</formula1>
+    </dataValidation>
+    <dataValidation sqref="B5" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A3:A7</formula1>
+    </dataValidation>
+    <dataValidation sqref="B6" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A3:A7</formula1>
+    </dataValidation>
+    <dataValidation sqref="C2" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A13:A16</formula1>
+    </dataValidation>
+    <dataValidation sqref="C3" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A13:A16</formula1>
+    </dataValidation>
+    <dataValidation sqref="C4" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A13:A16</formula1>
+    </dataValidation>
+    <dataValidation sqref="C5" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A13:A16</formula1>
+    </dataValidation>
+    <dataValidation sqref="C6" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A13:A16</formula1>
+    </dataValidation>
+    <dataValidation sqref="D2" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A22:A25</formula1>
+    </dataValidation>
+    <dataValidation sqref="D3" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A22:A25</formula1>
+    </dataValidation>
+    <dataValidation sqref="D4" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A22:A25</formula1>
+    </dataValidation>
+    <dataValidation sqref="D5" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A22:A25</formula1>
+    </dataValidation>
+    <dataValidation sqref="D6" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A22:A25</formula1>
+    </dataValidation>
+    <dataValidation sqref="E2" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A31:A34</formula1>
+    </dataValidation>
+    <dataValidation sqref="E3" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A31:A34</formula1>
+    </dataValidation>
+    <dataValidation sqref="E4" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A31:A34</formula1>
+    </dataValidation>
+    <dataValidation sqref="E5" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A31:A34</formula1>
+    </dataValidation>
+    <dataValidation sqref="E6" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A31:A34</formula1>
+    </dataValidation>
+    <dataValidation sqref="F2" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A40:A44</formula1>
+    </dataValidation>
+    <dataValidation sqref="F3" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A40:A44</formula1>
+    </dataValidation>
+    <dataValidation sqref="F4" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A40:A44</formula1>
+    </dataValidation>
+    <dataValidation sqref="F5" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A40:A44</formula1>
+    </dataValidation>
+    <dataValidation sqref="F6" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A40:A44</formula1>
+    </dataValidation>
+    <dataValidation sqref="G2" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A50:A53</formula1>
+    </dataValidation>
+    <dataValidation sqref="G3" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A50:A53</formula1>
+    </dataValidation>
+    <dataValidation sqref="G4" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A50:A53</formula1>
+    </dataValidation>
+    <dataValidation sqref="G5" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A50:A53</formula1>
+    </dataValidation>
+    <dataValidation sqref="G6" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A50:A53</formula1>
+    </dataValidation>
+    <dataValidation sqref="H2" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A59:A62</formula1>
+    </dataValidation>
+    <dataValidation sqref="H3" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A59:A62</formula1>
+    </dataValidation>
+    <dataValidation sqref="H4" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A59:A62</formula1>
+    </dataValidation>
+    <dataValidation sqref="H5" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A59:A62</formula1>
+    </dataValidation>
+    <dataValidation sqref="H6" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A59:A62</formula1>
+    </dataValidation>
     <dataValidation sqref="B2" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
       <formula1>=rating_scales!A3:A7</formula1>
     </dataValidation>

</xml_diff>